<commit_message>
changes to naming convention sheet
</commit_message>
<xml_diff>
--- a/final report/code/rules of function naming.xlsx
+++ b/final report/code/rules of function naming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscar/Desktop/uni/year-3/indiv project/finalproject/final report/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CB85A6-65BD-934A-83D7-D1B6CA61CA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057FF9EE-8C04-6D4A-A6C3-1CD1D91A9650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" xr2:uid="{FEE1AB29-80D8-E642-9307-0612689E39FB}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>related to training models</t>
   </si>
   <si>
-    <t>Eval</t>
-  </si>
-  <si>
     <t>VIS</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>any specific to imports, libraries, models, data</t>
+  </si>
+  <si>
+    <t>EVAL</t>
   </si>
 </sst>
 </file>
@@ -156,8 +156,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF73F90C-7F43-1A49-9E18-7C76109D4D40}" name="Table2" displayName="Table2" ref="A1:C10" totalsRowShown="0">
   <autoFilter ref="A1:C10" xr:uid="{EF73F90C-7F43-1A49-9E18-7C76109D4D40}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C9">
-    <sortCondition ref="A1:A9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C10">
+    <sortCondition ref="A1:A10"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{7ECC3275-DC21-934E-94D9-8F5F4E876020}" name="level of imporance"/>
@@ -488,7 +488,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="236" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,10 +558,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -569,10 +569,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -580,32 +580,32 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>